<commit_message>
standardize Excel tools : make clear where is INPUT and OUTPUT, plays with colors to help, ...
</commit_message>
<xml_diff>
--- a/tools/quizizz2aiken.xlsx
+++ b/tools/quizizz2aiken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apps\laragon\www\q4eef\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EBD2A7-8B39-4786-9F1B-039D2F073838}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8274D9D5-FA52-4B7B-A9F7-A072CB285E3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
   <si>
     <t>Multiple Choice</t>
   </si>
@@ -43,9 +43,6 @@
     <t>the first</t>
   </si>
   <si>
-    <t>AIKEN.TXT</t>
-  </si>
-  <si>
     <t>AIKEN.EXCEL</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>ANSWER:</t>
   </si>
   <si>
-    <t>EXCEL QUIZZIZ</t>
-  </si>
-  <si>
     <t>good answer</t>
   </si>
   <si>
@@ -77,22 +71,26 @@
   </si>
   <si>
     <t>copy-paste the cells from Exc el Quizizz in line 2</t>
+  </si>
+  <si>
+    <t>OUTPUT : AIKEN.TXT</t>
+  </si>
+  <si>
+    <t>INPUT EXCEL : QUIZZIZ</t>
+  </si>
+  <si>
+    <t>INTERMEDIATE RESULTS</t>
+  </si>
+  <si>
+    <t>***</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -114,6 +112,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
@@ -144,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -152,27 +167,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFFFFFF"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFFFFFF"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -187,29 +189,44 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="45" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="45" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="45" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
@@ -551,214 +568,493 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{808A41C4-4EBA-470E-A06E-EF08AFC23F0A}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="70.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1.157407407407407E-4</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+    </row>
+    <row r="6" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+    </row>
+    <row r="8" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+    </row>
+    <row r="9" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9">
-        <v>94</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="11">
-        <v>1.157407407407407E-4</v>
-      </c>
-      <c r="F2" s="9">
-        <v>1</v>
-      </c>
-      <c r="G2" s="9">
-        <v>0</v>
-      </c>
-      <c r="H2" s="9">
-        <v>0</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+    </row>
+    <row r="10" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="11" t="str">
+        <f>TRIM(CLEAN(I4))</f>
+        <v>all</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="str">
+        <f>B4</f>
+        <v>Progress Poker helps to ensure that _____ checklist item(s) is/are considered.</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="9" t="str">
+        <f>TRIM(CLEAN(K4))</f>
+        <v>all</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="9" t="str">
+        <f>TRIM(CLEAN(L4))</f>
+        <v>some</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="9" t="str">
+        <f>TRIM(CLEAN(M4))</f>
+        <v>the last</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="9" t="str">
+        <f>TRIM(CLEAN(N4))</f>
+        <v>the first</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="9" t="str">
+        <f>IF(B10=TRIM(B13),"A",IF(B10=B14,"B",IF(B10=B15,"C",IF(B10=B16,"D","ERREUR"))))</f>
+        <v>A</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="16" t="str">
-        <f>TRIM(CLEAN(I2))</f>
-        <v>all</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="str">
-        <f>B2</f>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="str">
+        <f>A12</f>
         <v>Progress Poker helps to ensure that _____ checklist item(s) is/are considered.</v>
       </c>
-      <c r="B8" s="14"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="14" t="str">
-        <f>TRIM(CLEAN(K2))</f>
-        <v>all</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="14" t="str">
-        <f>TRIM(CLEAN(L2))</f>
-        <v>some</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="14" t="str">
-        <f>TRIM(CLEAN(M2))</f>
-        <v>the last</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="14" t="str">
-        <f>TRIM(CLEAN(N2))</f>
-        <v>the first</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="14" t="str">
-        <f>IF(B5=TRIM(B9),"A",IF(B5=B10,"B",IF(B5=B11,"C",IF(B5=B12,"D","ERREUR"))))</f>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="str">
-        <f>A8</f>
-        <v>Progress Poker helps to ensure that _____ checklist item(s) is/are considered.</v>
-      </c>
-      <c r="B17" s="8"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="str">
-        <f>CONCATENATE(A9," ",B9)</f>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>CONCATENATE(A13," ",B13)</f>
         <v>A. all</v>
       </c>
-      <c r="B18" s="8"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="str">
-        <f>CONCATENATE(A10," ",B10)</f>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>CONCATENATE(A14," ",B14)</f>
         <v>B. some</v>
       </c>
-      <c r="B19" s="8"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="str">
-        <f t="shared" ref="A20:A22" si="0">CONCATENATE(A11," ",B11)</f>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f t="shared" ref="A26:A28" si="0">CONCATENATE(A15," ",B15)</f>
         <v>C. the last</v>
       </c>
-      <c r="B20" s="8"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="str">
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>D. the first</v>
       </c>
-      <c r="B21" s="8"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="str">
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>ANSWER: A</v>
       </c>
-      <c r="B22" s="8"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>